<commit_message>
Final version which result a usable JSON to upload in maximo.
</commit_message>
<xml_diff>
--- a/excel_file/uplaod_domain_name.xlsx
+++ b/excel_file/uplaod_domain_name.xlsx
@@ -5595,6 +5595,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5604,9 +5607,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5952,7 +5952,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5968,7 +5968,7 @@
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6982,7 +6982,7 @@
       <c r="A5" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="B5" s="83"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="54" t="s">
         <v>20</v>
       </c>
@@ -7092,7 +7092,7 @@
       <c r="A11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="83"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="54"/>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
@@ -7202,7 +7202,7 @@
       <c r="A17" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="83"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="51" t="s">
         <v>38</v>
       </c>
@@ -7297,7 +7297,7 @@
       <c r="A22" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="83"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="51"/>
       <c r="D22" s="51"/>
       <c r="E22" s="51"/>
@@ -7405,7 +7405,7 @@
       <c r="A28" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="83"/>
+      <c r="B28" s="80"/>
       <c r="C28" s="51"/>
       <c r="D28" s="51"/>
       <c r="E28" s="51"/>
@@ -7437,7 +7437,7 @@
       <c r="A30" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="83"/>
+      <c r="B30" s="80"/>
       <c r="C30" s="51"/>
       <c r="D30" s="51" t="s">
         <v>1058</v>
@@ -7769,7 +7769,7 @@
       <c r="A48" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="83"/>
+      <c r="B48" s="80"/>
       <c r="C48" s="51"/>
       <c r="D48" s="54"/>
       <c r="E48" s="51"/>
@@ -8047,7 +8047,7 @@
       <c r="A60" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B60" s="83"/>
+      <c r="B60" s="80"/>
       <c r="C60" s="51" t="s">
         <v>20</v>
       </c>
@@ -8229,7 +8229,7 @@
       <c r="A68" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="83"/>
+      <c r="B68" s="80"/>
       <c r="C68" s="51"/>
       <c r="D68" s="51"/>
       <c r="E68" s="51"/>
@@ -8331,7 +8331,7 @@
       <c r="A73" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B73" s="83"/>
+      <c r="B73" s="80"/>
       <c r="C73" s="51"/>
       <c r="D73" s="51"/>
       <c r="E73" s="51"/>
@@ -8461,7 +8461,7 @@
       <c r="A79" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B79" s="83"/>
+      <c r="B79" s="80"/>
       <c r="C79" s="51"/>
       <c r="D79" s="51" t="s">
         <v>20</v>
@@ -8575,7 +8575,7 @@
       <c r="A84" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="B84" s="83"/>
+      <c r="B84" s="80"/>
       <c r="C84" s="51"/>
       <c r="D84" s="51"/>
       <c r="E84" s="51"/>
@@ -8723,7 +8723,7 @@
       <c r="A91" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B91" s="83"/>
+      <c r="B91" s="80"/>
       <c r="C91" s="51"/>
       <c r="D91" s="51"/>
       <c r="E91" s="51"/>
@@ -8858,7 +8858,7 @@
       <c r="A98" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B98" s="83"/>
+      <c r="B98" s="80"/>
       <c r="C98" s="51"/>
       <c r="D98" s="51"/>
       <c r="E98" s="51"/>
@@ -9020,7 +9020,7 @@
       <c r="A108" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B108" s="83"/>
+      <c r="B108" s="80"/>
       <c r="C108" s="51"/>
       <c r="D108" s="51"/>
       <c r="E108" s="51"/>
@@ -9206,7 +9206,7 @@
       <c r="A118" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B118" s="83"/>
+      <c r="B118" s="80"/>
       <c r="C118" s="51"/>
       <c r="D118" s="51"/>
       <c r="E118" s="51"/>
@@ -9292,7 +9292,7 @@
       <c r="A122" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="B122" s="83"/>
+      <c r="B122" s="80"/>
       <c r="C122" s="64" t="s">
         <v>20</v>
       </c>
@@ -9463,7 +9463,7 @@
       <c r="A131" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="B131" s="83"/>
+      <c r="B131" s="80"/>
       <c r="C131" s="51"/>
       <c r="D131" s="51"/>
       <c r="E131" s="51"/>
@@ -9805,7 +9805,7 @@
       <c r="A147" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B147" s="83"/>
+      <c r="B147" s="80"/>
       <c r="C147" s="51"/>
       <c r="D147" s="51"/>
       <c r="E147" s="51"/>
@@ -10225,7 +10225,7 @@
       <c r="A166" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B166" s="83"/>
+      <c r="B166" s="80"/>
       <c r="C166" s="51"/>
       <c r="D166" s="51"/>
       <c r="E166" s="51"/>
@@ -10529,7 +10529,7 @@
       <c r="A184" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="B184" s="83"/>
+      <c r="B184" s="80"/>
       <c r="C184" s="50"/>
       <c r="D184" s="50"/>
       <c r="E184" s="50"/>
@@ -11326,7 +11326,7 @@
       <c r="A223" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B223" s="83"/>
+      <c r="B223" s="80"/>
       <c r="C223" s="51" t="s">
         <v>454</v>
       </c>
@@ -11686,7 +11686,7 @@
       <c r="A243" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B243" s="83"/>
+      <c r="B243" s="80"/>
       <c r="C243" s="9"/>
       <c r="D243" s="51"/>
       <c r="E243" s="51"/>
@@ -11977,7 +11977,7 @@
       <c r="A255" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B255" s="83"/>
+      <c r="B255" s="80"/>
       <c r="C255" s="51"/>
       <c r="D255" s="50"/>
       <c r="E255" s="50"/>
@@ -12077,7 +12077,7 @@
       <c r="A260" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B260" s="83"/>
+      <c r="B260" s="80"/>
       <c r="C260" s="51"/>
       <c r="D260" s="51"/>
       <c r="E260" s="51"/>
@@ -12207,7 +12207,7 @@
       <c r="A266" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B266" s="83"/>
+      <c r="B266" s="80"/>
       <c r="C266" s="51" t="s">
         <v>20</v>
       </c>
@@ -12421,10 +12421,10 @@
       <c r="L276" s="51"/>
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A277" s="84" t="s">
+      <c r="A277" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="B277" s="85"/>
+      <c r="B277" s="82"/>
       <c r="C277" s="51"/>
       <c r="D277" s="51"/>
       <c r="E277" s="51"/>
@@ -13103,10 +13103,10 @@
       <c r="L301" s="51"/>
     </row>
     <row r="302" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A302" s="84" t="s">
+      <c r="A302" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="B302" s="85"/>
+      <c r="B302" s="82"/>
       <c r="C302" s="51" t="s">
         <v>20</v>
       </c>
@@ -13256,10 +13256,10 @@
       <c r="L309" s="32"/>
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A310" s="84" t="s">
+      <c r="A310" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="B310" s="85"/>
+      <c r="B310" s="82"/>
       <c r="C310" s="51"/>
       <c r="D310" s="51"/>
       <c r="E310" s="51"/>
@@ -13405,7 +13405,7 @@
       <c r="A318" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B318" s="83"/>
+      <c r="B318" s="80"/>
       <c r="C318" s="51"/>
       <c r="D318" s="51"/>
       <c r="E318" s="51"/>
@@ -13556,7 +13556,7 @@
       <c r="A326" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B326" s="83"/>
+      <c r="B326" s="80"/>
       <c r="C326" s="11" t="s">
         <v>234</v>
       </c>
@@ -13663,7 +13663,7 @@
       <c r="A331" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B331" s="83"/>
+      <c r="B331" s="80"/>
       <c r="C331" s="11"/>
       <c r="D331" s="51"/>
       <c r="E331" s="51"/>
@@ -13806,7 +13806,7 @@
       <c r="A340" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B340" s="83"/>
+      <c r="B340" s="80"/>
       <c r="C340" s="11"/>
       <c r="D340" s="51"/>
       <c r="E340" s="51"/>
@@ -14098,7 +14098,7 @@
       <c r="A354" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="B354" s="83"/>
+      <c r="B354" s="80"/>
       <c r="C354" s="51" t="s">
         <v>20</v>
       </c>
@@ -14192,7 +14192,7 @@
       <c r="A358" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B358" s="83"/>
+      <c r="B358" s="80"/>
       <c r="C358" s="50" t="s">
         <v>20</v>
       </c>
@@ -14691,7 +14691,7 @@
       <c r="A379" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B379" s="83"/>
+      <c r="B379" s="80"/>
       <c r="C379" s="51"/>
       <c r="D379" s="51"/>
       <c r="E379" s="51"/>
@@ -14978,7 +14978,7 @@
       <c r="A395" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B395" s="83"/>
+      <c r="B395" s="80"/>
       <c r="C395" s="51"/>
       <c r="D395" s="51"/>
       <c r="E395" s="51"/>
@@ -15167,7 +15167,7 @@
       <c r="A405" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B405" s="83"/>
+      <c r="B405" s="80"/>
       <c r="C405" s="51"/>
       <c r="D405" s="51"/>
       <c r="E405" s="51"/>
@@ -15272,7 +15272,7 @@
       <c r="A410" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B410" s="83"/>
+      <c r="B410" s="80"/>
       <c r="C410" s="51"/>
       <c r="D410" s="51"/>
       <c r="E410" s="51"/>
@@ -15474,7 +15474,7 @@
       <c r="A420" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B420" s="83"/>
+      <c r="B420" s="80"/>
       <c r="C420" s="51" t="s">
         <v>1320</v>
       </c>
@@ -15570,7 +15570,7 @@
       <c r="A424" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B424" s="83"/>
+      <c r="B424" s="80"/>
       <c r="C424" s="51"/>
       <c r="D424" s="51"/>
       <c r="E424" s="51"/>
@@ -15680,13 +15680,13 @@
     <row r="428" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A428" s="62"/>
       <c r="B428" s="63"/>
-      <c r="C428" s="80" t="s">
+      <c r="C428" s="83" t="s">
         <v>709</v>
       </c>
-      <c r="D428" s="80" t="s">
+      <c r="D428" s="83" t="s">
         <v>709</v>
       </c>
-      <c r="E428" s="80" t="s">
+      <c r="E428" s="83" t="s">
         <v>709</v>
       </c>
       <c r="F428" s="51" t="s">
@@ -15708,9 +15708,9 @@
     <row r="429" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A429" s="62"/>
       <c r="B429" s="63"/>
-      <c r="C429" s="81"/>
-      <c r="D429" s="81"/>
-      <c r="E429" s="81"/>
+      <c r="C429" s="84"/>
+      <c r="D429" s="84"/>
+      <c r="E429" s="84"/>
       <c r="F429" s="51" t="s">
         <v>358</v>
       </c>
@@ -15730,9 +15730,9 @@
     <row r="430" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A430" s="62"/>
       <c r="B430" s="63"/>
-      <c r="C430" s="82"/>
-      <c r="D430" s="82"/>
-      <c r="E430" s="82"/>
+      <c r="C430" s="85"/>
+      <c r="D430" s="85"/>
+      <c r="E430" s="85"/>
       <c r="F430" s="51" t="s">
         <v>361</v>
       </c>
@@ -15852,7 +15852,7 @@
       <c r="A437" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B437" s="83"/>
+      <c r="B437" s="80"/>
       <c r="C437" s="51"/>
       <c r="D437" s="51"/>
       <c r="E437" s="51"/>
@@ -16191,7 +16191,7 @@
       <c r="A456" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B456" s="83"/>
+      <c r="B456" s="80"/>
       <c r="C456" s="51" t="s">
         <v>381</v>
       </c>
@@ -16305,7 +16305,7 @@
       <c r="A462" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B462" s="83"/>
+      <c r="B462" s="80"/>
       <c r="C462" s="51"/>
       <c r="D462" s="51"/>
       <c r="E462" s="51"/>
@@ -16421,7 +16421,7 @@
       <c r="A468" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B468" s="83"/>
+      <c r="B468" s="80"/>
       <c r="C468" s="51"/>
       <c r="D468" s="51"/>
       <c r="E468" s="51"/>
@@ -16891,7 +16891,7 @@
       <c r="A491" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="B491" s="83"/>
+      <c r="B491" s="80"/>
       <c r="C491" s="51"/>
       <c r="D491" s="64"/>
       <c r="E491" s="64"/>
@@ -16995,7 +16995,7 @@
       <c r="A496" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B496" s="83"/>
+      <c r="B496" s="80"/>
       <c r="C496" s="64"/>
       <c r="D496" s="64"/>
       <c r="E496" s="64"/>
@@ -17094,7 +17094,7 @@
       <c r="A501" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B501" s="83"/>
+      <c r="B501" s="80"/>
       <c r="C501" s="51" t="s">
         <v>20</v>
       </c>
@@ -17229,7 +17229,7 @@
       <c r="A508" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B508" s="83"/>
+      <c r="B508" s="80"/>
       <c r="C508" s="64"/>
       <c r="D508" s="64"/>
       <c r="E508" s="64"/>
@@ -17322,7 +17322,7 @@
       <c r="A513" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B513" s="83"/>
+      <c r="B513" s="80"/>
       <c r="C513" s="51"/>
       <c r="D513" s="51" t="s">
         <v>20</v>
@@ -17404,7 +17404,7 @@
       <c r="A517" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B517" s="83"/>
+      <c r="B517" s="80"/>
       <c r="C517" s="64"/>
       <c r="D517" s="64"/>
       <c r="E517" s="64"/>
@@ -17722,7 +17722,7 @@
       <c r="A533" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B533" s="83"/>
+      <c r="B533" s="80"/>
       <c r="C533" s="64"/>
       <c r="D533" s="56"/>
       <c r="E533" s="45" t="s">
@@ -17862,7 +17862,7 @@
       <c r="A541" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B541" s="83"/>
+      <c r="B541" s="80"/>
       <c r="C541" s="64"/>
       <c r="D541" s="56"/>
       <c r="E541" s="41"/>
@@ -18010,7 +18010,7 @@
       <c r="A549" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B549" s="83"/>
+      <c r="B549" s="80"/>
       <c r="C549" s="64"/>
       <c r="D549" s="56"/>
       <c r="E549" s="41"/>
@@ -18141,7 +18141,7 @@
       <c r="A556" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B556" s="83"/>
+      <c r="B556" s="80"/>
       <c r="C556" s="64" t="s">
         <v>1344</v>
       </c>
@@ -18414,7 +18414,7 @@
       <c r="A569" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B569" s="83"/>
+      <c r="B569" s="80"/>
       <c r="C569" s="64" t="s">
         <v>20</v>
       </c>
@@ -19039,7 +19039,7 @@
       <c r="A603" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B603" s="83"/>
+      <c r="B603" s="80"/>
       <c r="C603" s="57" t="s">
         <v>945</v>
       </c>
@@ -19138,7 +19138,7 @@
       <c r="A608" s="20" t="s">
         <v>1277</v>
       </c>
-      <c r="B608" s="83"/>
+      <c r="B608" s="80"/>
       <c r="C608" s="57"/>
       <c r="D608" s="64" t="s">
         <v>1033</v>
@@ -19313,7 +19313,7 @@
       <c r="A619" s="20" t="s">
         <v>1277</v>
       </c>
-      <c r="B619" s="83"/>
+      <c r="B619" s="80"/>
       <c r="C619" s="57"/>
       <c r="D619" s="64"/>
       <c r="E619" s="64"/>
@@ -19481,7 +19481,7 @@
       <c r="A627" s="20" t="s">
         <v>1277</v>
       </c>
-      <c r="B627" s="83"/>
+      <c r="B627" s="80"/>
       <c r="C627" s="64"/>
       <c r="D627" s="64"/>
       <c r="E627" s="49"/>
@@ -19645,7 +19645,7 @@
       <c r="A635" s="20" t="s">
         <v>1277</v>
       </c>
-      <c r="B635" s="83"/>
+      <c r="B635" s="80"/>
       <c r="C635" s="64"/>
       <c r="D635" s="64"/>
       <c r="E635" s="49"/>
@@ -19988,7 +19988,7 @@
       <c r="A651" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B651" s="83"/>
+      <c r="B651" s="80"/>
       <c r="C651" s="64"/>
       <c r="D651" s="64"/>
       <c r="E651" s="56"/>
@@ -20057,7 +20057,7 @@
       <c r="A654" s="20" t="s">
         <v>1277</v>
       </c>
-      <c r="B654" s="83"/>
+      <c r="B654" s="80"/>
       <c r="C654" s="64"/>
       <c r="D654" s="64"/>
       <c r="E654" s="56"/>
@@ -20210,7 +20210,7 @@
       <c r="A662" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B662" s="83"/>
+      <c r="B662" s="80"/>
       <c r="C662" s="64"/>
       <c r="D662" s="64"/>
       <c r="E662" s="64"/>
@@ -20304,7 +20304,7 @@
       <c r="A667" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B667" s="83"/>
+      <c r="B667" s="80"/>
       <c r="C667" s="64"/>
       <c r="D667" s="61"/>
       <c r="E667" s="64"/>
@@ -20471,7 +20471,7 @@
       <c r="A677" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B677" s="83"/>
+      <c r="B677" s="80"/>
       <c r="C677" s="64"/>
       <c r="D677" s="64"/>
       <c r="E677" s="56"/>
@@ -20550,7 +20550,7 @@
       <c r="A681" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B681" s="83"/>
+      <c r="B681" s="80"/>
       <c r="C681" s="64"/>
       <c r="D681" s="64"/>
       <c r="E681" s="56"/>
@@ -20669,7 +20669,7 @@
       <c r="A687" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B687" s="83"/>
+      <c r="B687" s="80"/>
       <c r="C687" s="64"/>
       <c r="D687" s="56"/>
       <c r="E687" s="64"/>
@@ -20832,7 +20832,7 @@
       <c r="A695" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B695" s="83"/>
+      <c r="B695" s="80"/>
       <c r="C695" s="64"/>
       <c r="D695" s="64"/>
       <c r="E695" s="56"/>
@@ -20967,7 +20967,7 @@
       <c r="A701" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B701" s="83"/>
+      <c r="B701" s="80"/>
       <c r="C701" s="64"/>
       <c r="D701" s="62"/>
       <c r="E701" s="64"/>
@@ -21132,7 +21132,7 @@
       <c r="A709" s="20" t="s">
         <v>1277</v>
       </c>
-      <c r="B709" s="83"/>
+      <c r="B709" s="80"/>
       <c r="C709" s="64"/>
       <c r="D709" s="64"/>
       <c r="E709" s="64"/>
@@ -21207,7 +21207,7 @@
       <c r="A712" s="20" t="s">
         <v>1277</v>
       </c>
-      <c r="B712" s="83"/>
+      <c r="B712" s="80"/>
       <c r="C712" s="64"/>
       <c r="D712" s="56"/>
       <c r="E712" s="56"/>
@@ -21297,7 +21297,7 @@
       <c r="A716" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B716" s="83"/>
+      <c r="B716" s="80"/>
       <c r="C716" s="64"/>
       <c r="D716" s="40" t="s">
         <v>20</v>
@@ -21381,7 +21381,7 @@
       <c r="A720" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B720" s="83"/>
+      <c r="B720" s="80"/>
       <c r="C720" s="64"/>
       <c r="D720" s="56"/>
       <c r="E720" s="56"/>
@@ -21547,7 +21547,7 @@
       <c r="A728" s="20" t="s">
         <v>1277</v>
       </c>
-      <c r="B728" s="83"/>
+      <c r="B728" s="80"/>
       <c r="C728" s="64"/>
       <c r="D728" s="62"/>
       <c r="E728" s="56"/>
@@ -21817,7 +21817,7 @@
       <c r="A744" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B744" s="83"/>
+      <c r="B744" s="80"/>
       <c r="C744" s="64"/>
       <c r="D744" s="64"/>
       <c r="E744" s="56"/>
@@ -21950,7 +21950,7 @@
       <c r="A751" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B751" s="83"/>
+      <c r="B751" s="80"/>
       <c r="C751" s="56"/>
       <c r="D751" s="56"/>
       <c r="E751" s="56"/>
@@ -22068,7 +22068,7 @@
       <c r="A757" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B757" s="83"/>
+      <c r="B757" s="80"/>
       <c r="C757" s="56"/>
       <c r="D757" s="56"/>
       <c r="E757" s="56"/>
@@ -22288,7 +22288,7 @@
       <c r="A769" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B769" s="83"/>
+      <c r="B769" s="80"/>
       <c r="C769" s="64"/>
       <c r="D769" s="64"/>
       <c r="E769" s="56"/>
@@ -22370,7 +22370,7 @@
       <c r="A773" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B773" s="83"/>
+      <c r="B773" s="80"/>
       <c r="C773" s="75"/>
       <c r="D773" s="75" t="s">
         <v>20</v>
@@ -22452,7 +22452,7 @@
       <c r="A777" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B777" s="83"/>
+      <c r="B777" s="80"/>
       <c r="C777" s="64"/>
       <c r="D777" s="64"/>
       <c r="E777" s="56"/>
@@ -22589,7 +22589,7 @@
       <c r="A784" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B784" s="83"/>
+      <c r="B784" s="80"/>
       <c r="C784" s="64"/>
       <c r="D784" s="64"/>
       <c r="E784" s="56"/>
@@ -22696,7 +22696,7 @@
       <c r="A789" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B789" s="83"/>
+      <c r="B789" s="80"/>
       <c r="C789" s="64"/>
       <c r="D789" s="64"/>
       <c r="E789" s="64"/>
@@ -22761,7 +22761,7 @@
       <c r="A792" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B792" s="83"/>
+      <c r="B792" s="80"/>
       <c r="C792" s="64"/>
       <c r="D792" s="64" t="s">
         <v>20</v>
@@ -22842,7 +22842,7 @@
       <c r="A795" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B795" s="83"/>
+      <c r="B795" s="80"/>
       <c r="C795" s="64"/>
       <c r="D795" s="64" t="s">
         <v>20</v>
@@ -22916,7 +22916,7 @@
       <c r="A798" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B798" s="83"/>
+      <c r="B798" s="80"/>
       <c r="C798" s="64"/>
       <c r="D798" s="64"/>
       <c r="E798" s="64"/>

</xml_diff>

<commit_message>
add trim() to account for weird spaces that user entered incorrectly:
</commit_message>
<xml_diff>
--- a/excel_file/uplaod_domain_name.xlsx
+++ b/excel_file/uplaod_domain_name.xlsx
@@ -570,7 +570,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2740" uniqueCount="1357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2738" uniqueCount="1357">
   <si>
     <t>Electrical</t>
   </si>
@@ -5966,9 +5966,9 @@
   <dimension ref="A1:O878"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="C264" sqref="C264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12075,7 +12075,7 @@
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260" s="20" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B260" s="80"/>
       <c r="C260" s="51"/>
@@ -12120,9 +12120,7 @@
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A262" s="62" t="s">
-        <v>20</v>
-      </c>
+      <c r="A262" s="62"/>
       <c r="B262" s="63"/>
       <c r="C262" s="51" t="s">
         <v>278</v>
@@ -12147,9 +12145,7 @@
       <c r="B263" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C263" s="51" t="s">
-        <v>20</v>
-      </c>
+      <c r="C263" s="51"/>
       <c r="D263" s="51" t="s">
         <v>841</v>
       </c>

</xml_diff>